<commit_message>
update output in rangefinder
</commit_message>
<xml_diff>
--- a/RANGE-FINDER-NODE/RANGE-FINDER-NODE/Project Outputs for RANGE-FINDER-NODE/BOM/Bill of Materials-BOM.xlsx
+++ b/RANGE-FINDER-NODE/RANGE-FINDER-NODE/Project Outputs for RANGE-FINDER-NODE/BOM/Bill of Materials-BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\UAV-CAN-MODULES\RANGE-FINDER-NODE\RANGE-FINDER-NODE\Project Outputs for RANGE-FINDER-NODE\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\altium workspace\UAV-CAN-MODULES\RANGE-FINDER-NODE\RANGE-FINDER-NODE\Project Outputs for RANGE-FINDER-NODE\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEEAB31A-7014-4976-980D-51ECB7F50D04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9F7BE22-60AF-41C6-8AD2-AA179FB89939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10125" xr2:uid="{014C6BA1-C6F4-4513-B00B-95C5260240D6}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{A1E5A39D-C6D7-41DC-8DE4-AC5B7219D660}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-BOM" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Bill of Materials-BOM'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -463,6 +463,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -515,7 +516,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -531,9 +532,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -571,7 +572,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -677,7 +678,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -826,7 +827,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF420A3-E01C-463F-B107-9A8517B494F1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{328CA351-571E-46F4-893A-BB3B56A819D5}">
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1705,6 +1706,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>